<commit_message>
finished outages by region and future planned outages
</commit_message>
<xml_diff>
--- a/Daily Data/OUTPUT/COAL/outages_20250313.xlsx
+++ b/Daily Data/OUTPUT/COAL/outages_20250313.xlsx
@@ -645,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I33"/>
+  <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
@@ -794,7 +794,7 @@
     <row r="10">
       <c r="B10" s="27" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>QLD</t>
         </is>
       </c>
       <c r="C10" s="24" t="n"/>
@@ -806,493 +806,122 @@
       <c r="I10" s="32" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="27" t="n"/>
-      <c r="C11" s="24" t="inlineStr">
-        <is>
-          <t>Bayswater 2</t>
-        </is>
-      </c>
-      <c r="D11" s="24" t="inlineStr">
+      <c r="B11" s="33" t="n"/>
+      <c r="C11" s="34" t="inlineStr">
+        <is>
+          <t>Gladstone 5</t>
+        </is>
+      </c>
+      <c r="D11" s="34" t="inlineStr">
         <is>
           <t>Existing</t>
         </is>
       </c>
-      <c r="E11" s="25" t="n">
-        <v>685</v>
-      </c>
-      <c r="F11" s="24" t="inlineStr">
-        <is>
-          <t>Unplanned</t>
-        </is>
-      </c>
-      <c r="G11" s="25" t="n">
-        <v>186</v>
-      </c>
-      <c r="H11" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I11" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
+      <c r="E11" s="35" t="n">
+        <v>280</v>
+      </c>
+      <c r="F11" s="34" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="G11" s="35" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" s="36" t="n">
+        <v>45732</v>
+      </c>
+      <c r="I11" s="37" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="27" t="n"/>
-      <c r="C12" s="24" t="inlineStr">
-        <is>
-          <t>Eraring 3</t>
-        </is>
-      </c>
-      <c r="D12" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E12" s="25" t="n">
-        <v>720</v>
-      </c>
-      <c r="F12" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G12" s="25" t="n">
-        <v>200</v>
-      </c>
-      <c r="H12" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I12" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Total planned</t>
+        </is>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>280</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="27" t="n"/>
-      <c r="C13" s="24" t="inlineStr">
-        <is>
-          <t>Vales Point B 6</t>
-        </is>
-      </c>
-      <c r="D13" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E13" s="25" t="n">
-        <v>660</v>
-      </c>
-      <c r="F13" s="24" t="inlineStr">
-        <is>
-          <t>Unplanned</t>
-        </is>
-      </c>
-      <c r="G13" s="25" t="n">
-        <v>169</v>
-      </c>
-      <c r="H13" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I13" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
+      <c r="B13" s="5" t="n"/>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Total unplanned</t>
+        </is>
+      </c>
+      <c r="D13" s="22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="27" t="inlineStr">
-        <is>
-          <t>QLD</t>
-        </is>
-      </c>
-      <c r="C14" s="24" t="n"/>
-      <c r="D14" s="24" t="n"/>
-      <c r="E14" s="25" t="n"/>
-      <c r="F14" s="24" t="n"/>
-      <c r="G14" s="25" t="n"/>
-      <c r="H14" s="26" t="n"/>
-      <c r="I14" s="32" t="n"/>
+      <c r="B14" s="5" t="n"/>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>Total unclear</t>
+        </is>
+      </c>
+      <c r="D14" s="23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="27" t="n"/>
-      <c r="C15" s="24" t="inlineStr">
-        <is>
-          <t>Callide B 1</t>
-        </is>
-      </c>
-      <c r="D15" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E15" s="25" t="n">
-        <v>350</v>
-      </c>
-      <c r="F15" s="24" t="inlineStr">
-        <is>
-          <t>Unplanned</t>
-        </is>
-      </c>
-      <c r="G15" s="25" t="n">
-        <v>238</v>
-      </c>
-      <c r="H15" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I15" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
+      <c r="B15" s="5" t="n"/>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>Total outages:</t>
+        </is>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>280</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="27" t="n"/>
-      <c r="C16" s="24" t="inlineStr">
-        <is>
-          <t>Callide B 2</t>
-        </is>
-      </c>
-      <c r="D16" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E16" s="25" t="n">
-        <v>350</v>
-      </c>
-      <c r="F16" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G16" s="25" t="n">
-        <v>182</v>
-      </c>
-      <c r="H16" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I16" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
+      <c r="B16" s="4" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="27" t="n"/>
-      <c r="C17" s="24" t="inlineStr">
-        <is>
-          <t>Gladstone 2</t>
-        </is>
-      </c>
-      <c r="D17" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E17" s="25" t="n">
-        <v>280</v>
-      </c>
-      <c r="F17" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G17" s="25" t="n">
-        <v>150</v>
-      </c>
-      <c r="H17" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I17" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>Returning coal units</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="27" t="n"/>
-      <c r="C18" s="24" t="inlineStr">
-        <is>
-          <t>Gladstone 6</t>
-        </is>
-      </c>
-      <c r="D18" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E18" s="25" t="n">
-        <v>280</v>
-      </c>
-      <c r="F18" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G18" s="25" t="n">
-        <v>172</v>
-      </c>
-      <c r="H18" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I18" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>Coal units returning to service after being offline on 12 March 2025:</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="24" t="inlineStr">
-        <is>
-          <t>Tarong 2</t>
-        </is>
-      </c>
-      <c r="D19" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E19" s="25" t="n">
-        <v>350</v>
-      </c>
-      <c r="F19" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G19" s="25" t="n">
-        <v>181</v>
-      </c>
-      <c r="H19" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I19" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
+      <c r="B19" s="9" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="inlineStr">
+        <is>
+          <t>Nameplate capacity (MW)</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>Days unit was unavailable</t>
         </is>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="27" t="inlineStr">
-        <is>
-          <t>VIC</t>
-        </is>
-      </c>
-      <c r="C20" s="24" t="n"/>
-      <c r="D20" s="24" t="n"/>
-      <c r="E20" s="25" t="n"/>
-      <c r="F20" s="24" t="n"/>
-      <c r="G20" s="25" t="n"/>
-      <c r="H20" s="26" t="n"/>
-      <c r="I20" s="32" t="n"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="27" t="n"/>
-      <c r="C21" s="24" t="inlineStr">
-        <is>
-          <t>Loy Yang A 2</t>
-        </is>
-      </c>
-      <c r="D21" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E21" s="25" t="n">
-        <v>530</v>
-      </c>
-      <c r="F21" s="24" t="inlineStr">
-        <is>
-          <t>Unplanned</t>
-        </is>
-      </c>
-      <c r="G21" s="25" t="n">
-        <v>154</v>
-      </c>
-      <c r="H21" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I21" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="24" t="inlineStr">
-        <is>
-          <t>Loy Yang A 4</t>
-        </is>
-      </c>
-      <c r="D22" s="24" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E22" s="25" t="n">
-        <v>560</v>
-      </c>
-      <c r="F22" s="24" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G22" s="25" t="n">
-        <v>164</v>
-      </c>
-      <c r="H22" s="26" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I22" s="32" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="33" t="n"/>
-      <c r="C23" s="34" t="inlineStr">
-        <is>
-          <t>Yallourn W 2</t>
-        </is>
-      </c>
-      <c r="D23" s="34" t="inlineStr">
-        <is>
-          <t>Existing</t>
-        </is>
-      </c>
-      <c r="E23" s="35" t="n">
-        <v>350</v>
-      </c>
-      <c r="F23" s="34" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G23" s="35" t="n">
-        <v>154</v>
-      </c>
-      <c r="H23" s="36" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="I23" s="37" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="31" t="n"/>
-      <c r="C24" s="5" t="inlineStr">
-        <is>
-          <t>Total planned</t>
-        </is>
-      </c>
-      <c r="D24" s="22" t="n">
-        <v>2890</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="5" t="n"/>
-      <c r="C25" s="5" t="inlineStr">
-        <is>
-          <t>Total unplanned</t>
-        </is>
-      </c>
-      <c r="D25" s="22" t="n">
-        <v>2225</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="5" t="n"/>
-      <c r="C26" s="6" t="inlineStr">
-        <is>
-          <t>Total unclear</t>
-        </is>
-      </c>
-      <c r="D26" s="23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="5" t="n"/>
-      <c r="C27" s="7" t="inlineStr">
-        <is>
-          <t>Total outages:</t>
-        </is>
-      </c>
-      <c r="D27" s="21" t="n">
-        <v>5115</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>Returning coal units</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>Coal units returning to service after being offline on 12 March 2025:</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="9" t="inlineStr">
-        <is>
-          <t>Unit</t>
-        </is>
-      </c>
-      <c r="C31" s="10" t="inlineStr">
-        <is>
-          <t>Nameplate capacity (MW)</t>
-        </is>
-      </c>
-      <c r="D31" s="11" t="inlineStr">
-        <is>
-          <t>Days unit was unavailable</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="18" t="n"/>
-      <c r="C32" s="19" t="n"/>
-      <c r="D32" s="20" t="n"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="4" t="n"/>
-    </row>
+      <c r="B20" s="18" t="n"/>
+      <c r="C20" s="19" t="n"/>
+      <c r="D20" s="20" t="n"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="B21" s="4" t="n"/>
+    </row>
+    <row r="22" ht="24" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="B5:H5">
     <cfRule type="colorScale" priority="1">

</xml_diff>